<commit_message>
feat(importer): EPI-1161: Importer to properly report on 'updated' records (#7858)
* feat(importer): Importer to properly report on 'updated' records

* update testing

* feat(importer): add new columns for skipped, deleted, and restored records in ImporterView

* fix(importer): Update ImporterView to reflect 'No change' for skipped records and include skipped in stat summation

* fix(importer): Improve handling of skipped records and update statistics accordingly

* fix(importer): Add configuration to ignore specific fields when checking for changes in importRows
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/programs-obsolete.xlsx
+++ b/packages/central-server/__tests__/importers/programs-obsolete.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="28800" windowHeight="11440"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Metadata" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Field types" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Samoa PEN Referral Example" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Ignored" sheetId="4" r:id="rId7"/>
+    <sheet name="Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Field types" sheetId="2" r:id="rId2"/>
+    <sheet name="Samoa PEN Referral Example" sheetId="3" r:id="rId3"/>
+    <sheet name="Ignored" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mjche8Ws6PKKc1VeI+RmkTOvavDdQ=="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -24,7 +22,7 @@
     <t>programName</t>
   </si>
   <si>
-    <t>Tamanu test suite program</t>
+    <t>Tamanu test suite program 2</t>
   </si>
   <si>
     <t>programCode</t>
@@ -84,7 +82,7 @@
     <t>Test-tonga</t>
   </si>
   <si>
-    <t>Samoa PEN Referral Example</t>
+    <t>Samoa PEN Referral Example 2</t>
   </si>
   <si>
     <t>obsolete</t>
@@ -534,78 +532,704 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -795,121 +1419,123 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.2205882352941" defaultRowHeight="15" customHeight="1" outlineLevelCol="6"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.44"/>
-    <col customWidth="1" min="2" max="2" width="29.89"/>
-    <col customWidth="1" min="3" max="6" width="19.22"/>
-    <col customWidth="1" min="7" max="7" width="10.44"/>
+    <col min="1" max="1" width="19.4411764705882" customWidth="1"/>
+    <col min="2" max="2" width="29.8897058823529" customWidth="1"/>
+    <col min="3" max="6" width="19.2205882352941" customWidth="1"/>
+    <col min="7" max="7" width="10.4411764705882" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="12.75" customHeight="1" spans="1:2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="12.75" customHeight="1" spans="1:2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="12.75" customHeight="1" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="12.75" customHeight="1" spans="1:1">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
-    <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="12.75" customHeight="1" spans="1:7">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="12.75" customHeight="1" spans="1:7">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="1" t="b">
+      <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="12.75" customHeight="1" spans="1:7">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="1" t="b">
+      <c r="G8" s="3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1906,305 +2532,304 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.2205882352941" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.44"/>
-    <col customWidth="1" min="2" max="2" width="27.56"/>
-    <col customWidth="1" min="3" max="3" width="10.44"/>
-    <col customWidth="1" min="4" max="4" width="27.44"/>
-    <col customWidth="1" min="5" max="15" width="10.44"/>
+    <col min="1" max="1" width="10.4411764705882" customWidth="1"/>
+    <col min="2" max="2" width="27.5588235294118" customWidth="1"/>
+    <col min="3" max="3" width="10.4411764705882" customWidth="1"/>
+    <col min="4" max="4" width="27.4411764705882" customWidth="1"/>
+    <col min="5" max="15" width="10.4411764705882" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="14.8" spans="1:15">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="14.8" spans="1:4">
+      <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="14.8" spans="1:2">
+      <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="14.8" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="14.8" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="14.8" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="14.8" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="14.8" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+    <row r="9" ht="14.8" spans="1:2">
+      <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+    <row r="10" ht="14.8" spans="1:2">
+      <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+    <row r="11" ht="14.8" spans="1:2">
+      <c r="A11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+    <row r="12" ht="14.8" spans="1:2">
+      <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+    <row r="13" ht="14.8" spans="1:2">
+      <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+    <row r="14" ht="14.8" spans="1:2">
+      <c r="A14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+    <row r="15" ht="14.8" spans="1:2">
+      <c r="A15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+    <row r="16" ht="14.8" spans="1:2">
+      <c r="A16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+    <row r="17" ht="14.8" spans="1:2">
+      <c r="A17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+    <row r="18" ht="14.8" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+    <row r="19" ht="14.8" spans="1:2">
+      <c r="A19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+    <row r="20" ht="14.8" spans="1:2">
+      <c r="A20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
+    <row r="21" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="22" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="23" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="24" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A24" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
+    <row r="25" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
+    <row r="26" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+    <row r="27" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+    <row r="28" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A28" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
+    <row r="29" ht="15.75" customHeight="1" spans="1:2">
+      <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3180,95 +3805,94 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.2205882352941" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.56"/>
-    <col customWidth="1" min="2" max="2" width="9.44"/>
-    <col customWidth="1" min="3" max="3" width="40.0"/>
-    <col customWidth="1" min="4" max="4" width="86.33"/>
-    <col customWidth="1" min="5" max="16" width="8.67"/>
+    <col min="1" max="1" width="30.5588235294118" customWidth="1"/>
+    <col min="2" max="2" width="9.44117647058824" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="86.3308823529412" customWidth="1"/>
+    <col min="5" max="16" width="8.66911764705882" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="30" spans="1:16">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="30" spans="1:16">
+      <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E2" s="2"/>
@@ -3284,17 +3908,17 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E3" s="2"/>
@@ -3310,17 +3934,17 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+    <row r="4" ht="134" spans="1:16">
+      <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>101</v>
       </c>
       <c r="E4" s="2"/>
@@ -3334,24 +3958,24 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+    <row r="5" ht="60" spans="1:16">
+      <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>105</v>
       </c>
       <c r="F5" s="2"/>
@@ -3366,20 +3990,20 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="60" spans="1:16">
+      <c r="A6" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F6" s="2"/>
@@ -3392,24 +4016,24 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+    <row r="7" ht="60" spans="1:16">
+      <c r="A7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F7" s="2"/>
@@ -3422,24 +4046,24 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
+    <row r="8" ht="60" spans="1:16">
+      <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F8" s="2"/>
@@ -3452,28 +4076,28 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+    <row r="9" ht="237" spans="1:16">
+      <c r="A9" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="1" t="s">
         <v>122</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>123</v>
       </c>
       <c r="H9" s="2"/>
@@ -3486,22 +4110,22 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+    <row r="10" ht="282" spans="1:16">
+      <c r="A10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="1" t="s">
         <v>126</v>
       </c>
       <c r="H10" s="2"/>
@@ -3514,20 +4138,20 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
+    <row r="11" ht="60" spans="1:16">
+      <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="1" t="s">
         <v>129</v>
       </c>
       <c r="F11" s="2"/>
@@ -3540,24 +4164,24 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
+    <row r="12" ht="60" spans="1:16">
+      <c r="A12" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="1" t="s">
         <v>129</v>
       </c>
       <c r="F12" s="2"/>
@@ -3570,24 +4194,24 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+    <row r="13" ht="30" spans="1:16">
+      <c r="A13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="1" t="s">
         <v>136</v>
       </c>
       <c r="F13" s="2"/>
@@ -3602,17 +4226,17 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+    <row r="14" ht="60" spans="1:16">
+      <c r="A14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E14" s="2"/>
@@ -3626,21 +4250,21 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="4" t="s">
+      <c r="P14" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+    <row r="15" ht="60" spans="1:16">
+      <c r="A15" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E15" s="2"/>
@@ -3654,24 +4278,24 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+    <row r="16" ht="30" spans="1:16">
+      <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F16" s="2"/>
@@ -3686,17 +4310,17 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+    <row r="17" ht="134" spans="1:16">
+      <c r="A17" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E17" s="2"/>
@@ -3710,24 +4334,24 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="4" t="s">
+      <c r="P17" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+    <row r="18" ht="89" spans="1:16">
+      <c r="A18" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="1" t="s">
         <v>152</v>
       </c>
       <c r="F18" s="2"/>
@@ -3742,27 +4366,27 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+    <row r="19" ht="89" spans="1:16">
+      <c r="A19" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="1" t="s">
         <v>156</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="1" t="s">
         <v>157</v>
       </c>
       <c r="K19" s="2"/>
@@ -3770,21 +4394,21 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="4" t="s">
+      <c r="P19" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+    <row r="20" ht="60" spans="1:16">
+      <c r="A20" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E20" s="2"/>
@@ -3792,7 +4416,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="1" t="s">
         <v>157</v>
       </c>
       <c r="K20" s="2"/>
@@ -3802,20 +4426,20 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+    <row r="21" ht="15.75" customHeight="1" spans="1:16">
+      <c r="A21" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="1" t="s">
         <v>165</v>
       </c>
       <c r="F21" s="2"/>
@@ -3830,20 +4454,20 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="4" t="s">
+    <row r="22" ht="15.75" customHeight="1" spans="1:16">
+      <c r="A22" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="1" t="s">
         <v>168</v>
       </c>
       <c r="F22" s="2"/>
@@ -3856,7 +4480,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="4" t="s">
+      <c r="P22" s="1" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4839,24 +5463,24 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.2205882352941" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="10.44"/>
+    <col min="1" max="6" width="10.4411764705882" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1"/>
@@ -5860,13 +6484,11 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>